<commit_message>
Updates to R2 with body functionality - add in open 2 inner doors, add body MD to full reset
</commit_message>
<xml_diff>
--- a/Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body/Dave Shadow Sounds.xlsx
+++ b/Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body/Dave Shadow Sounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\David\Documents\Droid Building\Audio\SHADOW Sounds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\David\Documents\GitHub\SHADOW\Shadow_Dave_MarcDuino_Warpdrives_UtilArms_2_0_Flithy_Body\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0A0712-E882-48E5-9B48-FB7F9878F910}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6065A2-C1C2-4CB4-9581-B0B9220BF9A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5160" yWindow="672" windowWidth="10488" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>L1/L2</t>
   </si>
   <si>
-    <t>Random Sounds</t>
-  </si>
-  <si>
     <t>Summer</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Fast Smirk (Dome Only)</t>
+  </si>
+  <si>
+    <t>Open 2 inner doors</t>
   </si>
 </sst>
 </file>
@@ -165,9 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +513,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +550,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -564,7 +567,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -575,13 +578,13 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -594,11 +597,11 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -618,7 +621,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -629,13 +632,13 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>